<commit_message>
seventh push by Somnath Baul
</commit_message>
<xml_diff>
--- a/TestSummary.xlsx
+++ b/TestSummary.xlsx
@@ -118,10 +118,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D2" t="n">
         <v>0.0</v>

</xml_diff>